<commit_message>
Most updated fwd flight data
</commit_message>
<xml_diff>
--- a/forward_flight.xlsx
+++ b/forward_flight.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hanh/GitHub/4343/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DA39ED-9FB0-A848-A7CF-EB0916A7C3C1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0C83C8-906E-104B-A8FE-95E25B6F195B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14020" xr2:uid="{DCD98145-CD71-A74D-B811-1F4E50135EAE}"/>
+    <workbookView xWindow="7500" yWindow="460" windowWidth="25040" windowHeight="14020" xr2:uid="{DCD98145-CD71-A74D-B811-1F4E50135EAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -53,13 +53,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,17 +61,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -130,28 +118,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="2" builtinId="10"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -466,7 +451,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +461,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -485,7 +470,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>208.33190701021078</v>
+        <v>178.30180551368241</v>
       </c>
       <c r="B2" s="2">
         <v>110</v>
@@ -493,7 +478,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>196.69264574485055</v>
+        <v>167.9995536168438</v>
       </c>
       <c r="B3" s="2">
         <v>115</v>
@@ -501,7 +486,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>187.00765931237152</v>
+        <v>159.38189133788265</v>
       </c>
       <c r="B4" s="2">
         <v>120</v>
@@ -509,7 +494,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>178.99273804137317</v>
+        <v>152.20245354675555</v>
       </c>
       <c r="B5" s="2">
         <v>125</v>
@@ -517,7 +502,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>172.41725449953603</v>
+        <v>146.26132249585379</v>
       </c>
       <c r="B6" s="2">
         <v>130</v>
@@ -525,7 +510,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>167.0924829724573</v>
+        <v>141.39490264339935</v>
       </c>
       <c r="B7" s="2">
         <v>135</v>
@@ -533,7 +518,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>162.86278514760451</v>
+        <v>137.46828002633853</v>
       </c>
       <c r="B8" s="2">
         <v>140</v>
@@ -541,7 +526,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>159.59888550641392</v>
+        <v>134.36939308186311</v>
       </c>
       <c r="B9" s="2">
         <v>145</v>
@@ -549,7 +534,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>157.19268881543491</v>
+        <v>132.00454022650871</v>
       </c>
       <c r="B10" s="2">
         <v>150</v>
@@ -557,7 +542,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>155.55324841291886</v>
+        <v>130.29488499409052</v>
       </c>
       <c r="B11" s="2">
         <v>155</v>
@@ -565,7 +550,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>154.60360224845064</v>
+        <v>129.17371337918624</v>
       </c>
       <c r="B12" s="2">
         <v>160</v>
@@ -573,7 +558,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>154.27826960889141</v>
+        <v>128.58426389184271</v>
       </c>
       <c r="B13" s="2">
         <v>165</v>
@@ -581,7 +566,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>154.52125543760081</v>
+        <v>128.47799761590332</v>
       </c>
       <c r="B14" s="2">
         <v>170</v>
@@ -589,23 +574,23 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>155.28444793669857</v>
+        <v>128.81320918193796</v>
       </c>
       <c r="B15" s="2">
         <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>156.52632330801623</v>
-      </c>
-      <c r="B16" s="3">
+      <c r="A16">
+        <v>129.55390398115915</v>
+      </c>
+      <c r="B16">
         <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>158.21089214905214</v>
+        <v>130.66888485625759</v>
       </c>
       <c r="B17" s="2">
         <v>185</v>
@@ -613,111 +598,111 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>160.30683731833744</v>
+        <v>132.13100476613323</v>
       </c>
       <c r="B18" s="2">
         <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>162.78680451239373</v>
-      </c>
-      <c r="B19" s="2">
+      <c r="A19">
+        <v>133.91655182758191</v>
+      </c>
+      <c r="B19">
         <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>165.62681540437222</v>
-      </c>
-      <c r="B20" s="2">
+      <c r="A20">
+        <v>136.00474059870376</v>
+      </c>
+      <c r="B20">
         <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>168.80577972944047</v>
-      </c>
-      <c r="B21" s="2">
+      <c r="A21">
+        <v>138.37728913359408</v>
+      </c>
+      <c r="B21">
         <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <v>172.3050877002018</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="A22">
+        <v>141.01806567055226</v>
+      </c>
+      <c r="B22">
         <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <v>176.10826798527108</v>
-      </c>
-      <c r="B23" s="2">
+      <c r="A23">
+        <v>143.91279215324514</v>
+      </c>
+      <c r="B23">
         <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>180.20069946928643</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="3">
+        <v>147.0487943719256</v>
+      </c>
+      <c r="B24" s="3">
         <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>184.56936734204399</v>
-      </c>
-      <c r="B25" s="3">
+      <c r="A25">
+        <v>150.41479053103544</v>
+      </c>
+      <c r="B25">
         <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>189.20265589313857</v>
-      </c>
-      <c r="B26" s="2">
+      <c r="A26">
+        <v>154.00071163471534</v>
+      </c>
+      <c r="B26">
         <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>194.09017183237933</v>
-      </c>
-      <c r="B27" s="2">
+      <c r="A27">
+        <v>157.79754833336509</v>
+      </c>
+      <c r="B27">
         <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>199.22259310255288</v>
-      </c>
-      <c r="B28" s="2">
+      <c r="A28">
+        <v>161.79721986806337</v>
+      </c>
+      <c r="B28">
         <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>204.59153906593281</v>
-      </c>
-      <c r="B29" s="2">
+      <c r="A29">
+        <v>165.99246154266839</v>
+      </c>
+      <c r="B29">
         <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>210.18945867967926</v>
-      </c>
-      <c r="B30" s="2">
+      <c r="A30">
+        <v>170.37672778945876</v>
+      </c>
+      <c r="B30">
         <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>216.00953386659472</v>
+        <v>174.9441084067615</v>
       </c>
       <c r="B31" s="2">
         <v>255</v>
@@ -725,7 +710,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>222.04559576643774</v>
+        <v>179.68925596199932</v>
       </c>
       <c r="B32" s="2">
         <v>260</v>
@@ -733,7 +718,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>228.29205194227421</v>
+        <v>184.60732269103482</v>
       </c>
       <c r="B33" s="2">
         <v>265</v>
@@ -741,7 +726,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>234.74382293422775</v>
+        <v>189.69390550024062</v>
       </c>
       <c r="B34" s="2">
         <v>270</v>
@@ -749,7 +734,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>241.39628681360935</v>
+        <v>194.94499790364128</v>
       </c>
       <c r="B35" s="2">
         <v>275</v>
@@ -757,7 +742,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>248.24523060491612</v>
+        <v>200.35694791341913</v>
       </c>
       <c r="B36" s="2">
         <v>280</v>
@@ -765,7 +750,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>255.28680762040329</v>
+        <v>205.92642105569158</v>
       </c>
       <c r="B37" s="2">
         <v>285</v>
@@ -773,47 +758,47 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>262.5174998988619</v>
+        <v>211.65036781083293</v>
       </c>
       <c r="B38" s="2">
         <v>290</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <v>269.93408506247965</v>
-      </c>
-      <c r="B39" s="2">
+      <c r="A39">
+        <v>217.52599488358027</v>
+      </c>
+      <c r="B39">
         <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
-        <v>277.53360700770247</v>
-      </c>
-      <c r="B40" s="2">
+      <c r="A40">
+        <v>223.55073979661577</v>
+      </c>
+      <c r="B40">
         <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="4">
-        <v>285.31334993147254</v>
-      </c>
-      <c r="B41" s="4">
+      <c r="A41" s="3">
+        <v>229.72224837539554</v>
+      </c>
+      <c r="B41" s="3">
         <v>305</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>293.27081526600068</v>
-      </c>
-      <c r="B42" s="2">
+      <c r="A42">
+        <v>236.03835475422156</v>
+      </c>
+      <c r="B42">
         <v>310</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>301.40370115571704</v>
+        <v>242.49706358598283</v>
       </c>
       <c r="B43" s="2">
         <v>315</v>
@@ -821,7 +806,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>309.70988416115262</v>
+        <v>249.09653418229473</v>
       </c>
       <c r="B44" s="2">
         <v>320</v>
@@ -829,7 +814,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>318.1874029178091</v>
+        <v>255.83506634830687</v>
       </c>
       <c r="B45" s="2">
         <v>325</v>
@@ -837,7 +822,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>326.83444351487378</v>
+        <v>262.71108770834684</v>
       </c>
       <c r="B46" s="2">
         <v>330</v>
@@ -845,7 +830,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>335.64932638998289</v>
+        <v>269.72314234573821</v>
       </c>
       <c r="B47" s="2">
         <v>335</v>
@@ -853,7 +838,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>344.63049456300394</v>
+        <v>276.86988060333903</v>
       </c>
       <c r="B48" s="2">
         <v>340</v>
@@ -861,7 +846,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>353.77650305473372</v>
+        <v>284.15004991121532</v>
       </c>
       <c r="B49" s="2">
         <v>345</v>
@@ -869,23 +854,23 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>363.08600935607308</v>
+        <v>291.56248652491348</v>
       </c>
       <c r="B50" s="2">
         <v>350</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
-        <v>372.55776483016126</v>
-      </c>
-      <c r="B51" s="5">
+      <c r="A51" s="4">
+        <v>299.1061080724611</v>
+      </c>
+      <c r="B51" s="4">
         <v>355</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A51">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -893,13 +878,13 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2F8BFEA9-32A6-2E4E-8C2A-FB9977D69DA4}</x14:id>
+          <x14:id>{1234A93F-D13E-514A-97EA-E65A04035FBE}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B51">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -907,7 +892,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E7CD34A2-A473-ED4D-A226-4EE5CA8E223E}</x14:id>
+          <x14:id>{6D22C636-015B-D649-BDEE-5BC3A0DCC8F2}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -917,7 +902,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2F8BFEA9-32A6-2E4E-8C2A-FB9977D69DA4}">
+          <x14:cfRule type="dataBar" id="{1234A93F-D13E-514A-97EA-E65A04035FBE}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -930,7 +915,7 @@
           <xm:sqref>A2:A51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E7CD34A2-A473-ED4D-A226-4EE5CA8E223E}">
+          <x14:cfRule type="dataBar" id="{6D22C636-015B-D649-BDEE-5BC3A0DCC8F2}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>